<commit_message>
Fixed Casing and Spacing
</commit_message>
<xml_diff>
--- a/examples/eop_config/spreadsheets/example-classroom_seating_plan.xlsx
+++ b/examples/eop_config/spreadsheets/example-classroom_seating_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Programming\cpp\entity_organisation_program\examples\eop_config\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27499E8B-DA8E-49BF-9BC6-2F3C9FD44033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9560DF94-A5DE-4E59-9CA0-2CC88391CCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="855" activeTab="2" xr2:uid="{C9CC07CA-097F-41A1-ADA2-CA7DD700E42B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="855" xr2:uid="{C9CC07CA-097F-41A1-ADA2-CA7DD700E42B}"/>
   </bookViews>
   <sheets>
     <sheet name="district" sheetId="1" r:id="rId1"/>
@@ -1238,7 +1238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C6BAA5-37B3-470A-AA0A-11ED5B065C20}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView zoomScale="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
@@ -2825,7 +2825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5A72C2-BD47-49D9-BCA8-A1B80ED921AD}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>

</xml_diff>